<commit_message>
changed some stuff in test hydro 2
</commit_message>
<xml_diff>
--- a/eureca_dhcs/test/input_tests/conditions_hydro_test_2.xlsx
+++ b/eureca_dhcs/test/input_tests/conditions_hydro_test_2.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20386"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEA7EDD5-5679-4C68-B6E7-F38D39DDD36F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2BA47B5-9399-4550-8987-E957479B0E16}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15912" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16848" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hydraulic" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -83,7 +83,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -367,7 +367,7 @@
   <dimension ref="A1:J8763"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -458,27 +458,27 @@
       </c>
       <c r="B4" s="3">
         <f>-SUM(D4:G4)-C4</f>
-        <v>-103.70000000000002</v>
+        <v>-103.0778</v>
       </c>
       <c r="C4" s="3">
-        <f>-126.36/3.6</f>
-        <v>-35.1</v>
+        <f>-126.36/3.6*0.994</f>
+        <v>-34.889400000000002</v>
       </c>
       <c r="D4" s="3">
-        <f>113.4/3.6</f>
-        <v>31.5</v>
+        <f>113.4/3.6*0.994</f>
+        <v>31.311</v>
       </c>
       <c r="E4" s="3">
-        <f>90.72/3.6</f>
-        <v>25.2</v>
+        <f>90.72/3.6*0.994</f>
+        <v>25.0488</v>
       </c>
       <c r="F4" s="3">
-        <f>159.12/3.6</f>
-        <v>44.2</v>
+        <f>159.12/3.6*0.994</f>
+        <v>43.934800000000003</v>
       </c>
       <c r="G4" s="3">
-        <f>136.44/3.6</f>
-        <v>37.9</v>
+        <f>136.44/3.6*0.994</f>
+        <v>37.672599999999996</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
@@ -489,27 +489,27 @@
       </c>
       <c r="B5" s="3">
         <f t="shared" ref="B5:B6" si="0">-SUM(D5:G5)-C5</f>
-        <v>-103.70000000000002</v>
+        <v>-103.0778</v>
       </c>
       <c r="C5" s="3">
-        <f t="shared" ref="C5:C6" si="1">-126.36/3.6</f>
-        <v>-35.1</v>
+        <f t="shared" ref="C5:C6" si="1">-126.36/3.6*0.994</f>
+        <v>-34.889400000000002</v>
       </c>
       <c r="D5" s="3">
-        <f t="shared" ref="D5:D6" si="2">113.4/3.6</f>
-        <v>31.5</v>
+        <f t="shared" ref="D5:D6" si="2">113.4/3.6*0.994</f>
+        <v>31.311</v>
       </c>
       <c r="E5" s="3">
-        <f t="shared" ref="E5:E6" si="3">90.72/3.6</f>
-        <v>25.2</v>
+        <f t="shared" ref="E5:E6" si="3">90.72/3.6*0.994</f>
+        <v>25.0488</v>
       </c>
       <c r="F5" s="3">
-        <f t="shared" ref="F5:F6" si="4">159.12/3.6</f>
-        <v>44.2</v>
+        <f t="shared" ref="F5:F6" si="4">159.12/3.6*0.994</f>
+        <v>43.934800000000003</v>
       </c>
       <c r="G5" s="3">
-        <f t="shared" ref="G5:G6" si="5">136.44/3.6</f>
-        <v>37.9</v>
+        <f t="shared" ref="G5:G6" si="5">136.44/3.6*0.994</f>
+        <v>37.672599999999996</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
@@ -518,27 +518,27 @@
       </c>
       <c r="B6" s="3">
         <f t="shared" si="0"/>
-        <v>-103.70000000000002</v>
+        <v>-103.0778</v>
       </c>
       <c r="C6" s="3">
         <f t="shared" si="1"/>
-        <v>-35.1</v>
+        <v>-34.889400000000002</v>
       </c>
       <c r="D6" s="3">
         <f t="shared" si="2"/>
-        <v>31.5</v>
+        <v>31.311</v>
       </c>
       <c r="E6" s="3">
         <f t="shared" si="3"/>
-        <v>25.2</v>
+        <v>25.0488</v>
       </c>
       <c r="F6" s="3">
         <f t="shared" si="4"/>
-        <v>44.2</v>
+        <v>43.934800000000003</v>
       </c>
       <c r="G6" s="3">
         <f t="shared" si="5"/>
-        <v>37.9</v>
+        <v>37.672599999999996</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
changed the algorithm of optimization. more stable
</commit_message>
<xml_diff>
--- a/eureca_dhcs/test/input_tests/conditions_hydro_test_2.xlsx
+++ b/eureca_dhcs/test/input_tests/conditions_hydro_test_2.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20386"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2BA47B5-9399-4550-8987-E957479B0E16}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDB37DFA-D292-4367-BB1A-51FEC9C273AA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16848" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21528" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hydraulic" sheetId="1" r:id="rId1"/>
@@ -366,8 +366,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J8763"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -492,23 +492,23 @@
         <v>-103.0778</v>
       </c>
       <c r="C5" s="3">
-        <f t="shared" ref="C5:C6" si="1">-126.36/3.6*0.994</f>
+        <f t="shared" ref="C5:C15" si="1">-126.36/3.6*0.994</f>
         <v>-34.889400000000002</v>
       </c>
       <c r="D5" s="3">
-        <f t="shared" ref="D5:D6" si="2">113.4/3.6*0.994</f>
+        <f t="shared" ref="D5:D15" si="2">113.4/3.6*0.994</f>
         <v>31.311</v>
       </c>
       <c r="E5" s="3">
-        <f t="shared" ref="E5:E6" si="3">90.72/3.6*0.994</f>
+        <f t="shared" ref="E5:E15" si="3">90.72/3.6*0.994</f>
         <v>25.0488</v>
       </c>
       <c r="F5" s="3">
-        <f t="shared" ref="F5:F6" si="4">159.12/3.6*0.994</f>
+        <f t="shared" ref="F5:F15" si="4">159.12/3.6*0.994</f>
         <v>43.934800000000003</v>
       </c>
       <c r="G5" s="3">
-        <f t="shared" ref="G5:G6" si="5">136.44/3.6*0.994</f>
+        <f t="shared" ref="G5:G15" si="5">136.44/3.6*0.994</f>
         <v>37.672599999999996</v>
       </c>
     </row>
@@ -542,177 +542,1341 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="2"/>
+      <c r="A7" s="2">
+        <v>44198.083333159724</v>
+      </c>
+      <c r="B7" s="3">
+        <f t="shared" ref="B7:B15" si="6">-SUM(D7:G7)-C7</f>
+        <v>-103.0778</v>
+      </c>
+      <c r="C7" s="3">
+        <f t="shared" si="1"/>
+        <v>-34.889400000000002</v>
+      </c>
+      <c r="D7" s="3">
+        <f t="shared" si="2"/>
+        <v>31.311</v>
+      </c>
+      <c r="E7" s="3">
+        <f t="shared" si="3"/>
+        <v>25.0488</v>
+      </c>
+      <c r="F7" s="3">
+        <f t="shared" si="4"/>
+        <v>43.934800000000003</v>
+      </c>
+      <c r="G7" s="3">
+        <f t="shared" si="5"/>
+        <v>37.672599999999996</v>
+      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="2"/>
+      <c r="A8" s="2">
+        <v>44199.083333159724</v>
+      </c>
+      <c r="B8" s="3">
+        <f t="shared" si="6"/>
+        <v>-103.0778</v>
+      </c>
+      <c r="C8" s="3">
+        <f t="shared" si="1"/>
+        <v>-34.889400000000002</v>
+      </c>
+      <c r="D8" s="3">
+        <f t="shared" si="2"/>
+        <v>31.311</v>
+      </c>
+      <c r="E8" s="3">
+        <f t="shared" si="3"/>
+        <v>25.0488</v>
+      </c>
+      <c r="F8" s="3">
+        <f t="shared" si="4"/>
+        <v>43.934800000000003</v>
+      </c>
+      <c r="G8" s="3">
+        <f t="shared" si="5"/>
+        <v>37.672599999999996</v>
+      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="2"/>
+      <c r="A9" s="2">
+        <v>44200.083333159724</v>
+      </c>
+      <c r="B9" s="3">
+        <f t="shared" si="6"/>
+        <v>-103.0778</v>
+      </c>
+      <c r="C9" s="3">
+        <f t="shared" si="1"/>
+        <v>-34.889400000000002</v>
+      </c>
+      <c r="D9" s="3">
+        <f t="shared" si="2"/>
+        <v>31.311</v>
+      </c>
+      <c r="E9" s="3">
+        <f t="shared" si="3"/>
+        <v>25.0488</v>
+      </c>
+      <c r="F9" s="3">
+        <f t="shared" si="4"/>
+        <v>43.934800000000003</v>
+      </c>
+      <c r="G9" s="3">
+        <f t="shared" si="5"/>
+        <v>37.672599999999996</v>
+      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="2"/>
+      <c r="A10" s="2">
+        <v>44201.083333159724</v>
+      </c>
+      <c r="B10" s="3">
+        <f t="shared" si="6"/>
+        <v>-103.0778</v>
+      </c>
+      <c r="C10" s="3">
+        <f t="shared" si="1"/>
+        <v>-34.889400000000002</v>
+      </c>
+      <c r="D10" s="3">
+        <f t="shared" si="2"/>
+        <v>31.311</v>
+      </c>
+      <c r="E10" s="3">
+        <f t="shared" si="3"/>
+        <v>25.0488</v>
+      </c>
+      <c r="F10" s="3">
+        <f t="shared" si="4"/>
+        <v>43.934800000000003</v>
+      </c>
+      <c r="G10" s="3">
+        <f t="shared" si="5"/>
+        <v>37.672599999999996</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="2"/>
+      <c r="A11" s="2">
+        <v>44202.083333159724</v>
+      </c>
+      <c r="B11" s="3">
+        <f t="shared" si="6"/>
+        <v>-103.0778</v>
+      </c>
+      <c r="C11" s="3">
+        <f t="shared" si="1"/>
+        <v>-34.889400000000002</v>
+      </c>
+      <c r="D11" s="3">
+        <f t="shared" si="2"/>
+        <v>31.311</v>
+      </c>
+      <c r="E11" s="3">
+        <f t="shared" si="3"/>
+        <v>25.0488</v>
+      </c>
+      <c r="F11" s="3">
+        <f t="shared" si="4"/>
+        <v>43.934800000000003</v>
+      </c>
+      <c r="G11" s="3">
+        <f t="shared" si="5"/>
+        <v>37.672599999999996</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" s="2"/>
+      <c r="A12" s="2">
+        <v>44203.083333159724</v>
+      </c>
+      <c r="B12" s="3">
+        <f t="shared" si="6"/>
+        <v>-103.0778</v>
+      </c>
+      <c r="C12" s="3">
+        <f t="shared" si="1"/>
+        <v>-34.889400000000002</v>
+      </c>
+      <c r="D12" s="3">
+        <f t="shared" si="2"/>
+        <v>31.311</v>
+      </c>
+      <c r="E12" s="3">
+        <f t="shared" si="3"/>
+        <v>25.0488</v>
+      </c>
+      <c r="F12" s="3">
+        <f t="shared" si="4"/>
+        <v>43.934800000000003</v>
+      </c>
+      <c r="G12" s="3">
+        <f t="shared" si="5"/>
+        <v>37.672599999999996</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" s="2"/>
+      <c r="A13" s="2">
+        <v>44204.083333159724</v>
+      </c>
+      <c r="B13" s="3">
+        <f t="shared" si="6"/>
+        <v>-103.0778</v>
+      </c>
+      <c r="C13" s="3">
+        <f t="shared" si="1"/>
+        <v>-34.889400000000002</v>
+      </c>
+      <c r="D13" s="3">
+        <f t="shared" si="2"/>
+        <v>31.311</v>
+      </c>
+      <c r="E13" s="3">
+        <f t="shared" si="3"/>
+        <v>25.0488</v>
+      </c>
+      <c r="F13" s="3">
+        <f t="shared" si="4"/>
+        <v>43.934800000000003</v>
+      </c>
+      <c r="G13" s="3">
+        <f t="shared" si="5"/>
+        <v>37.672599999999996</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="2"/>
+      <c r="A14" s="2">
+        <v>44205.083333159724</v>
+      </c>
+      <c r="B14" s="3">
+        <f t="shared" si="6"/>
+        <v>-103.0778</v>
+      </c>
+      <c r="C14" s="3">
+        <f t="shared" si="1"/>
+        <v>-34.889400000000002</v>
+      </c>
+      <c r="D14" s="3">
+        <f t="shared" si="2"/>
+        <v>31.311</v>
+      </c>
+      <c r="E14" s="3">
+        <f t="shared" si="3"/>
+        <v>25.0488</v>
+      </c>
+      <c r="F14" s="3">
+        <f t="shared" si="4"/>
+        <v>43.934800000000003</v>
+      </c>
+      <c r="G14" s="3">
+        <f t="shared" si="5"/>
+        <v>37.672599999999996</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15" s="2"/>
+      <c r="A15" s="2">
+        <v>44206.083333159724</v>
+      </c>
+      <c r="B15" s="3">
+        <f t="shared" si="6"/>
+        <v>-103.0778</v>
+      </c>
+      <c r="C15" s="3">
+        <f t="shared" si="1"/>
+        <v>-34.889400000000002</v>
+      </c>
+      <c r="D15" s="3">
+        <f t="shared" si="2"/>
+        <v>31.311</v>
+      </c>
+      <c r="E15" s="3">
+        <f t="shared" si="3"/>
+        <v>25.0488</v>
+      </c>
+      <c r="F15" s="3">
+        <f t="shared" si="4"/>
+        <v>43.934800000000003</v>
+      </c>
+      <c r="G15" s="3">
+        <f t="shared" si="5"/>
+        <v>37.672599999999996</v>
+      </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" s="2"/>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" s="2"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" s="2"/>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" s="2"/>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20" s="2"/>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21" s="2"/>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A22" s="2"/>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A23" s="2"/>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A24" s="2"/>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A25" s="2"/>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A26" s="2"/>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A27" s="2"/>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A28" s="2"/>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A29" s="2"/>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A30" s="2"/>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A31" s="2"/>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A32" s="2"/>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A33" s="2"/>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A34" s="2"/>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A35" s="2"/>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A36" s="2"/>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A37" s="2"/>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A38" s="2"/>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A39" s="2"/>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A40" s="2"/>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A41" s="2"/>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A42" s="2"/>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A43" s="2"/>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A44" s="2"/>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A45" s="2"/>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A46" s="2"/>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A47" s="2"/>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A48" s="2"/>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A49" s="2"/>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A50" s="2"/>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A51" s="2"/>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A52" s="2"/>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A53" s="2"/>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A54" s="2"/>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16" s="2">
+        <v>44207.083333159724</v>
+      </c>
+      <c r="B16" s="3">
+        <v>0</v>
+      </c>
+      <c r="C16" s="3">
+        <v>0</v>
+      </c>
+      <c r="D16" s="3">
+        <v>0</v>
+      </c>
+      <c r="E16" s="3">
+        <v>0</v>
+      </c>
+      <c r="F16" s="3">
+        <v>0</v>
+      </c>
+      <c r="G16" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="2">
+        <v>44208.083333159724</v>
+      </c>
+      <c r="B17" s="3">
+        <v>0</v>
+      </c>
+      <c r="C17" s="3">
+        <v>0</v>
+      </c>
+      <c r="D17" s="3">
+        <v>0</v>
+      </c>
+      <c r="E17" s="3">
+        <v>0</v>
+      </c>
+      <c r="F17" s="3">
+        <v>0</v>
+      </c>
+      <c r="G17" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="2">
+        <v>44209.083333159724</v>
+      </c>
+      <c r="B18" s="3">
+        <v>0</v>
+      </c>
+      <c r="C18" s="3">
+        <v>0</v>
+      </c>
+      <c r="D18" s="3">
+        <v>0</v>
+      </c>
+      <c r="E18" s="3">
+        <v>0</v>
+      </c>
+      <c r="F18" s="3">
+        <v>0</v>
+      </c>
+      <c r="G18" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="2">
+        <v>44210.083333159724</v>
+      </c>
+      <c r="B19" s="3">
+        <v>0</v>
+      </c>
+      <c r="C19" s="3">
+        <v>0</v>
+      </c>
+      <c r="D19" s="3">
+        <v>0</v>
+      </c>
+      <c r="E19" s="3">
+        <v>0</v>
+      </c>
+      <c r="F19" s="3">
+        <v>0</v>
+      </c>
+      <c r="G19" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="2">
+        <v>44211.083333159724</v>
+      </c>
+      <c r="B20" s="3">
+        <v>0</v>
+      </c>
+      <c r="C20" s="3">
+        <v>0</v>
+      </c>
+      <c r="D20" s="3">
+        <v>0</v>
+      </c>
+      <c r="E20" s="3">
+        <v>0</v>
+      </c>
+      <c r="F20" s="3">
+        <v>0</v>
+      </c>
+      <c r="G20" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="2">
+        <v>44212.083333159724</v>
+      </c>
+      <c r="B21" s="3">
+        <v>0</v>
+      </c>
+      <c r="C21" s="3">
+        <v>0</v>
+      </c>
+      <c r="D21" s="3">
+        <v>0</v>
+      </c>
+      <c r="E21" s="3">
+        <v>0</v>
+      </c>
+      <c r="F21" s="3">
+        <v>0</v>
+      </c>
+      <c r="G21" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="2">
+        <v>44213.083333159724</v>
+      </c>
+      <c r="B22" s="3">
+        <v>0</v>
+      </c>
+      <c r="C22" s="3">
+        <v>0</v>
+      </c>
+      <c r="D22" s="3">
+        <v>0</v>
+      </c>
+      <c r="E22" s="3">
+        <v>0</v>
+      </c>
+      <c r="F22" s="3">
+        <v>0</v>
+      </c>
+      <c r="G22" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" s="2">
+        <v>44214.083333159724</v>
+      </c>
+      <c r="B23" s="3">
+        <v>0</v>
+      </c>
+      <c r="C23" s="3">
+        <v>0</v>
+      </c>
+      <c r="D23" s="3">
+        <v>0</v>
+      </c>
+      <c r="E23" s="3">
+        <v>0</v>
+      </c>
+      <c r="F23" s="3">
+        <v>0</v>
+      </c>
+      <c r="G23" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" s="2">
+        <v>44215.083333159724</v>
+      </c>
+      <c r="B24" s="3">
+        <v>0</v>
+      </c>
+      <c r="C24" s="3">
+        <v>0</v>
+      </c>
+      <c r="D24" s="3">
+        <v>0</v>
+      </c>
+      <c r="E24" s="3">
+        <v>0</v>
+      </c>
+      <c r="F24" s="3">
+        <v>0</v>
+      </c>
+      <c r="G24" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" s="2">
+        <v>44216.083333159724</v>
+      </c>
+      <c r="B25" s="3">
+        <v>0</v>
+      </c>
+      <c r="C25" s="3">
+        <v>0</v>
+      </c>
+      <c r="D25" s="3">
+        <v>0</v>
+      </c>
+      <c r="E25" s="3">
+        <v>0</v>
+      </c>
+      <c r="F25" s="3">
+        <v>0</v>
+      </c>
+      <c r="G25" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" s="2">
+        <v>44217.083333159724</v>
+      </c>
+      <c r="B26" s="3">
+        <v>0</v>
+      </c>
+      <c r="C26" s="3">
+        <v>0</v>
+      </c>
+      <c r="D26" s="3">
+        <v>0</v>
+      </c>
+      <c r="E26" s="3">
+        <v>0</v>
+      </c>
+      <c r="F26" s="3">
+        <v>0</v>
+      </c>
+      <c r="G26" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" s="2">
+        <v>44218.083333159724</v>
+      </c>
+      <c r="B27" s="3">
+        <v>0</v>
+      </c>
+      <c r="C27" s="3">
+        <v>0</v>
+      </c>
+      <c r="D27" s="3">
+        <v>0</v>
+      </c>
+      <c r="E27" s="3">
+        <v>0</v>
+      </c>
+      <c r="F27" s="3">
+        <v>0</v>
+      </c>
+      <c r="G27" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" s="2">
+        <v>44219.083333159724</v>
+      </c>
+      <c r="B28" s="3">
+        <v>0</v>
+      </c>
+      <c r="C28" s="3">
+        <v>0</v>
+      </c>
+      <c r="D28" s="3">
+        <v>0</v>
+      </c>
+      <c r="E28" s="3">
+        <v>0</v>
+      </c>
+      <c r="F28" s="3">
+        <v>0</v>
+      </c>
+      <c r="G28" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" s="2">
+        <v>44220.083333159724</v>
+      </c>
+      <c r="B29" s="3">
+        <v>0</v>
+      </c>
+      <c r="C29" s="3">
+        <v>0</v>
+      </c>
+      <c r="D29" s="3">
+        <v>0</v>
+      </c>
+      <c r="E29" s="3">
+        <v>0</v>
+      </c>
+      <c r="F29" s="3">
+        <v>0</v>
+      </c>
+      <c r="G29" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" s="2">
+        <v>44221.083333159724</v>
+      </c>
+      <c r="B30" s="3">
+        <f>-SUM(D30:G30)-C30</f>
+        <v>-241.14440000000005</v>
+      </c>
+      <c r="C30" s="3">
+        <f>-126.36/3.6*0.994</f>
+        <v>-34.889400000000002</v>
+      </c>
+      <c r="D30" s="3">
+        <f>113.4/3.6*0.994*2</f>
+        <v>62.622</v>
+      </c>
+      <c r="E30" s="3">
+        <f>90.72/3.6*0.994/2</f>
+        <v>12.5244</v>
+      </c>
+      <c r="F30" s="3">
+        <f>159.12/3.6*0.994*2</f>
+        <v>87.869600000000005</v>
+      </c>
+      <c r="G30" s="3">
+        <f>136.44/3.6*0.994*3</f>
+        <v>113.01779999999999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" s="2">
+        <v>44222.083333159724</v>
+      </c>
+      <c r="B31" s="3">
+        <f t="shared" ref="B31:B54" si="7">-SUM(D31:G31)-C31</f>
+        <v>-241.14440000000005</v>
+      </c>
+      <c r="C31" s="3">
+        <f t="shared" ref="C31:C54" si="8">-126.36/3.6*0.994</f>
+        <v>-34.889400000000002</v>
+      </c>
+      <c r="D31" s="3">
+        <f t="shared" ref="D31:D54" si="9">113.4/3.6*0.994*2</f>
+        <v>62.622</v>
+      </c>
+      <c r="E31" s="3">
+        <f t="shared" ref="E31:E54" si="10">90.72/3.6*0.994/2</f>
+        <v>12.5244</v>
+      </c>
+      <c r="F31" s="3">
+        <f t="shared" ref="F31:F54" si="11">159.12/3.6*0.994*2</f>
+        <v>87.869600000000005</v>
+      </c>
+      <c r="G31" s="3">
+        <f t="shared" ref="G31:G54" si="12">136.44/3.6*0.994*3</f>
+        <v>113.01779999999999</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" s="2">
+        <v>44223.083333159724</v>
+      </c>
+      <c r="B32" s="3">
+        <f t="shared" si="7"/>
+        <v>-241.14440000000005</v>
+      </c>
+      <c r="C32" s="3">
+        <f t="shared" si="8"/>
+        <v>-34.889400000000002</v>
+      </c>
+      <c r="D32" s="3">
+        <f t="shared" si="9"/>
+        <v>62.622</v>
+      </c>
+      <c r="E32" s="3">
+        <f t="shared" si="10"/>
+        <v>12.5244</v>
+      </c>
+      <c r="F32" s="3">
+        <f t="shared" si="11"/>
+        <v>87.869600000000005</v>
+      </c>
+      <c r="G32" s="3">
+        <f t="shared" si="12"/>
+        <v>113.01779999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33" s="2">
+        <v>44224.083333159724</v>
+      </c>
+      <c r="B33" s="3">
+        <f t="shared" si="7"/>
+        <v>-241.14440000000005</v>
+      </c>
+      <c r="C33" s="3">
+        <f t="shared" si="8"/>
+        <v>-34.889400000000002</v>
+      </c>
+      <c r="D33" s="3">
+        <f t="shared" si="9"/>
+        <v>62.622</v>
+      </c>
+      <c r="E33" s="3">
+        <f t="shared" si="10"/>
+        <v>12.5244</v>
+      </c>
+      <c r="F33" s="3">
+        <f t="shared" si="11"/>
+        <v>87.869600000000005</v>
+      </c>
+      <c r="G33" s="3">
+        <f t="shared" si="12"/>
+        <v>113.01779999999999</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34" s="2">
+        <v>44225.083333159724</v>
+      </c>
+      <c r="B34" s="3">
+        <f t="shared" si="7"/>
+        <v>-241.14440000000005</v>
+      </c>
+      <c r="C34" s="3">
+        <f t="shared" si="8"/>
+        <v>-34.889400000000002</v>
+      </c>
+      <c r="D34" s="3">
+        <f t="shared" si="9"/>
+        <v>62.622</v>
+      </c>
+      <c r="E34" s="3">
+        <f t="shared" si="10"/>
+        <v>12.5244</v>
+      </c>
+      <c r="F34" s="3">
+        <f t="shared" si="11"/>
+        <v>87.869600000000005</v>
+      </c>
+      <c r="G34" s="3">
+        <f t="shared" si="12"/>
+        <v>113.01779999999999</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35" s="2">
+        <v>44226.083333159724</v>
+      </c>
+      <c r="B35" s="3">
+        <f t="shared" si="7"/>
+        <v>-241.14440000000005</v>
+      </c>
+      <c r="C35" s="3">
+        <f t="shared" si="8"/>
+        <v>-34.889400000000002</v>
+      </c>
+      <c r="D35" s="3">
+        <f t="shared" si="9"/>
+        <v>62.622</v>
+      </c>
+      <c r="E35" s="3">
+        <f t="shared" si="10"/>
+        <v>12.5244</v>
+      </c>
+      <c r="F35" s="3">
+        <f t="shared" si="11"/>
+        <v>87.869600000000005</v>
+      </c>
+      <c r="G35" s="3">
+        <f t="shared" si="12"/>
+        <v>113.01779999999999</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36" s="2">
+        <v>44227.083333159724</v>
+      </c>
+      <c r="B36" s="3">
+        <f t="shared" si="7"/>
+        <v>-241.14440000000005</v>
+      </c>
+      <c r="C36" s="3">
+        <f t="shared" si="8"/>
+        <v>-34.889400000000002</v>
+      </c>
+      <c r="D36" s="3">
+        <f t="shared" si="9"/>
+        <v>62.622</v>
+      </c>
+      <c r="E36" s="3">
+        <f t="shared" si="10"/>
+        <v>12.5244</v>
+      </c>
+      <c r="F36" s="3">
+        <f t="shared" si="11"/>
+        <v>87.869600000000005</v>
+      </c>
+      <c r="G36" s="3">
+        <f t="shared" si="12"/>
+        <v>113.01779999999999</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A37" s="2">
+        <v>44228.083333159724</v>
+      </c>
+      <c r="B37" s="3">
+        <f t="shared" si="7"/>
+        <v>-241.14440000000005</v>
+      </c>
+      <c r="C37" s="3">
+        <f t="shared" si="8"/>
+        <v>-34.889400000000002</v>
+      </c>
+      <c r="D37" s="3">
+        <f t="shared" si="9"/>
+        <v>62.622</v>
+      </c>
+      <c r="E37" s="3">
+        <f t="shared" si="10"/>
+        <v>12.5244</v>
+      </c>
+      <c r="F37" s="3">
+        <f t="shared" si="11"/>
+        <v>87.869600000000005</v>
+      </c>
+      <c r="G37" s="3">
+        <f t="shared" si="12"/>
+        <v>113.01779999999999</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38" s="2">
+        <v>44229.083333159724</v>
+      </c>
+      <c r="B38" s="3">
+        <f t="shared" si="7"/>
+        <v>-241.14440000000005</v>
+      </c>
+      <c r="C38" s="3">
+        <f t="shared" si="8"/>
+        <v>-34.889400000000002</v>
+      </c>
+      <c r="D38" s="3">
+        <f t="shared" si="9"/>
+        <v>62.622</v>
+      </c>
+      <c r="E38" s="3">
+        <f t="shared" si="10"/>
+        <v>12.5244</v>
+      </c>
+      <c r="F38" s="3">
+        <f t="shared" si="11"/>
+        <v>87.869600000000005</v>
+      </c>
+      <c r="G38" s="3">
+        <f t="shared" si="12"/>
+        <v>113.01779999999999</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A39" s="2">
+        <v>44230.083333159724</v>
+      </c>
+      <c r="B39" s="3">
+        <f t="shared" si="7"/>
+        <v>-241.14440000000005</v>
+      </c>
+      <c r="C39" s="3">
+        <f t="shared" si="8"/>
+        <v>-34.889400000000002</v>
+      </c>
+      <c r="D39" s="3">
+        <f t="shared" si="9"/>
+        <v>62.622</v>
+      </c>
+      <c r="E39" s="3">
+        <f t="shared" si="10"/>
+        <v>12.5244</v>
+      </c>
+      <c r="F39" s="3">
+        <f t="shared" si="11"/>
+        <v>87.869600000000005</v>
+      </c>
+      <c r="G39" s="3">
+        <f t="shared" si="12"/>
+        <v>113.01779999999999</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A40" s="2">
+        <v>44231.083333159724</v>
+      </c>
+      <c r="B40" s="3">
+        <f t="shared" si="7"/>
+        <v>-241.14440000000005</v>
+      </c>
+      <c r="C40" s="3">
+        <f t="shared" si="8"/>
+        <v>-34.889400000000002</v>
+      </c>
+      <c r="D40" s="3">
+        <f t="shared" si="9"/>
+        <v>62.622</v>
+      </c>
+      <c r="E40" s="3">
+        <f t="shared" si="10"/>
+        <v>12.5244</v>
+      </c>
+      <c r="F40" s="3">
+        <f t="shared" si="11"/>
+        <v>87.869600000000005</v>
+      </c>
+      <c r="G40" s="3">
+        <f t="shared" si="12"/>
+        <v>113.01779999999999</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A41" s="2">
+        <v>44232.083333159724</v>
+      </c>
+      <c r="B41" s="3">
+        <f t="shared" si="7"/>
+        <v>-241.14440000000005</v>
+      </c>
+      <c r="C41" s="3">
+        <f t="shared" si="8"/>
+        <v>-34.889400000000002</v>
+      </c>
+      <c r="D41" s="3">
+        <f t="shared" si="9"/>
+        <v>62.622</v>
+      </c>
+      <c r="E41" s="3">
+        <f t="shared" si="10"/>
+        <v>12.5244</v>
+      </c>
+      <c r="F41" s="3">
+        <f t="shared" si="11"/>
+        <v>87.869600000000005</v>
+      </c>
+      <c r="G41" s="3">
+        <f t="shared" si="12"/>
+        <v>113.01779999999999</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A42" s="2">
+        <v>44233.083333159724</v>
+      </c>
+      <c r="B42" s="3">
+        <f t="shared" si="7"/>
+        <v>-241.14440000000005</v>
+      </c>
+      <c r="C42" s="3">
+        <f t="shared" si="8"/>
+        <v>-34.889400000000002</v>
+      </c>
+      <c r="D42" s="3">
+        <f t="shared" si="9"/>
+        <v>62.622</v>
+      </c>
+      <c r="E42" s="3">
+        <f t="shared" si="10"/>
+        <v>12.5244</v>
+      </c>
+      <c r="F42" s="3">
+        <f t="shared" si="11"/>
+        <v>87.869600000000005</v>
+      </c>
+      <c r="G42" s="3">
+        <f t="shared" si="12"/>
+        <v>113.01779999999999</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A43" s="2">
+        <v>44234.083333159724</v>
+      </c>
+      <c r="B43" s="3">
+        <f t="shared" si="7"/>
+        <v>-241.14440000000005</v>
+      </c>
+      <c r="C43" s="3">
+        <f t="shared" si="8"/>
+        <v>-34.889400000000002</v>
+      </c>
+      <c r="D43" s="3">
+        <f t="shared" si="9"/>
+        <v>62.622</v>
+      </c>
+      <c r="E43" s="3">
+        <f t="shared" si="10"/>
+        <v>12.5244</v>
+      </c>
+      <c r="F43" s="3">
+        <f t="shared" si="11"/>
+        <v>87.869600000000005</v>
+      </c>
+      <c r="G43" s="3">
+        <f t="shared" si="12"/>
+        <v>113.01779999999999</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A44" s="2">
+        <v>44235.083333159724</v>
+      </c>
+      <c r="B44" s="3">
+        <f t="shared" si="7"/>
+        <v>-222.35780000000003</v>
+      </c>
+      <c r="C44" s="3">
+        <f t="shared" si="8"/>
+        <v>-34.889400000000002</v>
+      </c>
+      <c r="D44" s="3">
+        <f>113.4/3.6*0.994</f>
+        <v>31.311</v>
+      </c>
+      <c r="E44" s="3">
+        <f>90.72/3.6*0.994</f>
+        <v>25.0488</v>
+      </c>
+      <c r="F44" s="3">
+        <f t="shared" si="11"/>
+        <v>87.869600000000005</v>
+      </c>
+      <c r="G44" s="3">
+        <f t="shared" si="12"/>
+        <v>113.01779999999999</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A45" s="2">
+        <v>44236.083333159724</v>
+      </c>
+      <c r="B45" s="3">
+        <f t="shared" si="7"/>
+        <v>-222.35780000000003</v>
+      </c>
+      <c r="C45" s="3">
+        <f t="shared" si="8"/>
+        <v>-34.889400000000002</v>
+      </c>
+      <c r="D45" s="3">
+        <f t="shared" ref="D45:D54" si="13">113.4/3.6*0.994</f>
+        <v>31.311</v>
+      </c>
+      <c r="E45" s="3">
+        <f t="shared" ref="E45:E54" si="14">90.72/3.6*0.994</f>
+        <v>25.0488</v>
+      </c>
+      <c r="F45" s="3">
+        <f t="shared" si="11"/>
+        <v>87.869600000000005</v>
+      </c>
+      <c r="G45" s="3">
+        <f t="shared" si="12"/>
+        <v>113.01779999999999</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A46" s="2">
+        <v>44237.083333159724</v>
+      </c>
+      <c r="B46" s="3">
+        <f t="shared" si="7"/>
+        <v>-222.35780000000003</v>
+      </c>
+      <c r="C46" s="3">
+        <f t="shared" si="8"/>
+        <v>-34.889400000000002</v>
+      </c>
+      <c r="D46" s="3">
+        <f t="shared" si="13"/>
+        <v>31.311</v>
+      </c>
+      <c r="E46" s="3">
+        <f t="shared" si="14"/>
+        <v>25.0488</v>
+      </c>
+      <c r="F46" s="3">
+        <f t="shared" si="11"/>
+        <v>87.869600000000005</v>
+      </c>
+      <c r="G46" s="3">
+        <f t="shared" si="12"/>
+        <v>113.01779999999999</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A47" s="2">
+        <v>44238.083333159724</v>
+      </c>
+      <c r="B47" s="3">
+        <f t="shared" si="7"/>
+        <v>-222.35780000000003</v>
+      </c>
+      <c r="C47" s="3">
+        <f t="shared" si="8"/>
+        <v>-34.889400000000002</v>
+      </c>
+      <c r="D47" s="3">
+        <f t="shared" si="13"/>
+        <v>31.311</v>
+      </c>
+      <c r="E47" s="3">
+        <f t="shared" si="14"/>
+        <v>25.0488</v>
+      </c>
+      <c r="F47" s="3">
+        <f t="shared" si="11"/>
+        <v>87.869600000000005</v>
+      </c>
+      <c r="G47" s="3">
+        <f t="shared" si="12"/>
+        <v>113.01779999999999</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A48" s="2">
+        <v>44239.083333159724</v>
+      </c>
+      <c r="B48" s="3">
+        <f t="shared" si="7"/>
+        <v>-222.35780000000003</v>
+      </c>
+      <c r="C48" s="3">
+        <f t="shared" si="8"/>
+        <v>-34.889400000000002</v>
+      </c>
+      <c r="D48" s="3">
+        <f t="shared" si="13"/>
+        <v>31.311</v>
+      </c>
+      <c r="E48" s="3">
+        <f t="shared" si="14"/>
+        <v>25.0488</v>
+      </c>
+      <c r="F48" s="3">
+        <f t="shared" si="11"/>
+        <v>87.869600000000005</v>
+      </c>
+      <c r="G48" s="3">
+        <f t="shared" si="12"/>
+        <v>113.01779999999999</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A49" s="2">
+        <v>44240.083333159724</v>
+      </c>
+      <c r="B49" s="3">
+        <f t="shared" si="7"/>
+        <v>-222.35780000000003</v>
+      </c>
+      <c r="C49" s="3">
+        <f t="shared" si="8"/>
+        <v>-34.889400000000002</v>
+      </c>
+      <c r="D49" s="3">
+        <f t="shared" si="13"/>
+        <v>31.311</v>
+      </c>
+      <c r="E49" s="3">
+        <f t="shared" si="14"/>
+        <v>25.0488</v>
+      </c>
+      <c r="F49" s="3">
+        <f t="shared" si="11"/>
+        <v>87.869600000000005</v>
+      </c>
+      <c r="G49" s="3">
+        <f t="shared" si="12"/>
+        <v>113.01779999999999</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A50" s="2">
+        <v>44241.083333159724</v>
+      </c>
+      <c r="B50" s="3">
+        <f t="shared" si="7"/>
+        <v>-222.35780000000003</v>
+      </c>
+      <c r="C50" s="3">
+        <f t="shared" si="8"/>
+        <v>-34.889400000000002</v>
+      </c>
+      <c r="D50" s="3">
+        <f t="shared" si="13"/>
+        <v>31.311</v>
+      </c>
+      <c r="E50" s="3">
+        <f t="shared" si="14"/>
+        <v>25.0488</v>
+      </c>
+      <c r="F50" s="3">
+        <f t="shared" si="11"/>
+        <v>87.869600000000005</v>
+      </c>
+      <c r="G50" s="3">
+        <f t="shared" si="12"/>
+        <v>113.01779999999999</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A51" s="2">
+        <v>44242.083333159724</v>
+      </c>
+      <c r="B51" s="3">
+        <f t="shared" si="7"/>
+        <v>-222.35780000000003</v>
+      </c>
+      <c r="C51" s="3">
+        <f t="shared" si="8"/>
+        <v>-34.889400000000002</v>
+      </c>
+      <c r="D51" s="3">
+        <f t="shared" si="13"/>
+        <v>31.311</v>
+      </c>
+      <c r="E51" s="3">
+        <f t="shared" si="14"/>
+        <v>25.0488</v>
+      </c>
+      <c r="F51" s="3">
+        <f t="shared" si="11"/>
+        <v>87.869600000000005</v>
+      </c>
+      <c r="G51" s="3">
+        <f t="shared" si="12"/>
+        <v>113.01779999999999</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A52" s="2">
+        <v>44243.083333159724</v>
+      </c>
+      <c r="B52" s="3">
+        <f t="shared" si="7"/>
+        <v>-222.35780000000003</v>
+      </c>
+      <c r="C52" s="3">
+        <f t="shared" si="8"/>
+        <v>-34.889400000000002</v>
+      </c>
+      <c r="D52" s="3">
+        <f t="shared" si="13"/>
+        <v>31.311</v>
+      </c>
+      <c r="E52" s="3">
+        <f t="shared" si="14"/>
+        <v>25.0488</v>
+      </c>
+      <c r="F52" s="3">
+        <f t="shared" si="11"/>
+        <v>87.869600000000005</v>
+      </c>
+      <c r="G52" s="3">
+        <f t="shared" si="12"/>
+        <v>113.01779999999999</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A53" s="2">
+        <v>44244.083333159724</v>
+      </c>
+      <c r="B53" s="3">
+        <f t="shared" si="7"/>
+        <v>-222.35780000000003</v>
+      </c>
+      <c r="C53" s="3">
+        <f t="shared" si="8"/>
+        <v>-34.889400000000002</v>
+      </c>
+      <c r="D53" s="3">
+        <f t="shared" si="13"/>
+        <v>31.311</v>
+      </c>
+      <c r="E53" s="3">
+        <f t="shared" si="14"/>
+        <v>25.0488</v>
+      </c>
+      <c r="F53" s="3">
+        <f t="shared" si="11"/>
+        <v>87.869600000000005</v>
+      </c>
+      <c r="G53" s="3">
+        <f t="shared" si="12"/>
+        <v>113.01779999999999</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A54" s="2">
+        <v>44245.083333159724</v>
+      </c>
+      <c r="B54" s="3">
+        <f t="shared" si="7"/>
+        <v>-222.35780000000003</v>
+      </c>
+      <c r="C54" s="3">
+        <f t="shared" si="8"/>
+        <v>-34.889400000000002</v>
+      </c>
+      <c r="D54" s="3">
+        <f t="shared" si="13"/>
+        <v>31.311</v>
+      </c>
+      <c r="E54" s="3">
+        <f t="shared" si="14"/>
+        <v>25.0488</v>
+      </c>
+      <c r="F54" s="3">
+        <f t="shared" si="11"/>
+        <v>87.869600000000005</v>
+      </c>
+      <c r="G54" s="3">
+        <f t="shared" si="12"/>
+        <v>113.01779999999999</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" s="2"/>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" s="2"/>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" s="2"/>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" s="2"/>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" s="2"/>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" s="2"/>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" s="2"/>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" s="2"/>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" s="2"/>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" s="2"/>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.3">
@@ -26822,8 +27986,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5227661-1F4F-4C60-9C9A-A070D4D4BCBF}">
   <dimension ref="A1:F8763"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -26906,177 +28070,561 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="2"/>
+      <c r="A7" s="2">
+        <v>44198.083333159724</v>
+      </c>
+      <c r="B7">
+        <v>20</v>
+      </c>
+      <c r="C7">
+        <v>20</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="2"/>
+      <c r="A8" s="2">
+        <v>44199.083333159724</v>
+      </c>
+      <c r="B8">
+        <v>20</v>
+      </c>
+      <c r="C8">
+        <v>20</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="2"/>
+      <c r="A9" s="2">
+        <v>44200.083333159724</v>
+      </c>
+      <c r="B9">
+        <v>20</v>
+      </c>
+      <c r="C9">
+        <v>20</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="2"/>
+      <c r="A10" s="2">
+        <v>44201.083333159724</v>
+      </c>
+      <c r="B10">
+        <v>20</v>
+      </c>
+      <c r="C10">
+        <v>20</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="2"/>
+      <c r="A11" s="2">
+        <v>44202.083333159724</v>
+      </c>
+      <c r="B11">
+        <v>20</v>
+      </c>
+      <c r="C11">
+        <v>20</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="2"/>
+      <c r="A12" s="2">
+        <v>44203.083333159724</v>
+      </c>
+      <c r="B12">
+        <v>20</v>
+      </c>
+      <c r="C12">
+        <v>20</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="2"/>
+      <c r="A13" s="2">
+        <v>44204.083333159724</v>
+      </c>
+      <c r="B13">
+        <v>20</v>
+      </c>
+      <c r="C13">
+        <v>20</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="2"/>
+      <c r="A14" s="2">
+        <v>44205.083333159724</v>
+      </c>
+      <c r="B14">
+        <v>20</v>
+      </c>
+      <c r="C14">
+        <v>20</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="2"/>
+      <c r="A15" s="2">
+        <v>44206.083333159724</v>
+      </c>
+      <c r="B15">
+        <v>20</v>
+      </c>
+      <c r="C15">
+        <v>20</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="2"/>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" s="2"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" s="2"/>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" s="2"/>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20" s="2"/>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21" s="2"/>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A22" s="2"/>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A23" s="2"/>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A24" s="2"/>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A25" s="2"/>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A26" s="2"/>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A27" s="2"/>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A28" s="2"/>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A29" s="2"/>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A30" s="2"/>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A31" s="2"/>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A32" s="2"/>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A33" s="2"/>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A34" s="2"/>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A35" s="2"/>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A36" s="2"/>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A37" s="2"/>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A38" s="2"/>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A39" s="2"/>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A40" s="2"/>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A41" s="2"/>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A42" s="2"/>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A43" s="2"/>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A44" s="2"/>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A45" s="2"/>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A46" s="2"/>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A47" s="2"/>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A48" s="2"/>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A49" s="2"/>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A50" s="2"/>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A51" s="2"/>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A52" s="2"/>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A53" s="2"/>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A54" s="2"/>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16" s="2">
+        <v>44207.083333159724</v>
+      </c>
+      <c r="B16">
+        <v>20</v>
+      </c>
+      <c r="C16">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="2">
+        <v>44208.083333159724</v>
+      </c>
+      <c r="B17">
+        <v>20</v>
+      </c>
+      <c r="C17">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="2">
+        <v>44209.083333159724</v>
+      </c>
+      <c r="B18">
+        <v>20</v>
+      </c>
+      <c r="C18">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="2">
+        <v>44210.083333159724</v>
+      </c>
+      <c r="B19">
+        <v>20</v>
+      </c>
+      <c r="C19">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="2">
+        <v>44211.083333159724</v>
+      </c>
+      <c r="B20">
+        <v>20</v>
+      </c>
+      <c r="C20">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="2">
+        <v>44212.083333159724</v>
+      </c>
+      <c r="B21">
+        <v>20</v>
+      </c>
+      <c r="C21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="2">
+        <v>44213.083333159724</v>
+      </c>
+      <c r="B22">
+        <v>20</v>
+      </c>
+      <c r="C22">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="2">
+        <v>44214.083333159724</v>
+      </c>
+      <c r="B23">
+        <v>20</v>
+      </c>
+      <c r="C23">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="2">
+        <v>44215.083333159724</v>
+      </c>
+      <c r="B24">
+        <v>20</v>
+      </c>
+      <c r="C24">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="2">
+        <v>44216.083333159724</v>
+      </c>
+      <c r="B25">
+        <v>20</v>
+      </c>
+      <c r="C25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="2">
+        <v>44217.083333159724</v>
+      </c>
+      <c r="B26">
+        <v>20</v>
+      </c>
+      <c r="C26">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="2">
+        <v>44218.083333159724</v>
+      </c>
+      <c r="B27">
+        <v>20</v>
+      </c>
+      <c r="C27">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="2">
+        <v>44219.083333159724</v>
+      </c>
+      <c r="B28">
+        <v>20</v>
+      </c>
+      <c r="C28">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="2">
+        <v>44220.083333159724</v>
+      </c>
+      <c r="B29">
+        <v>20</v>
+      </c>
+      <c r="C29">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="2">
+        <v>44221.083333159724</v>
+      </c>
+      <c r="B30">
+        <v>20</v>
+      </c>
+      <c r="C30">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="2">
+        <v>44222.083333159724</v>
+      </c>
+      <c r="B31">
+        <v>20</v>
+      </c>
+      <c r="C31">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="2">
+        <v>44223.083333159724</v>
+      </c>
+      <c r="B32">
+        <v>20</v>
+      </c>
+      <c r="C32">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="2">
+        <v>44224.083333159724</v>
+      </c>
+      <c r="B33">
+        <v>20</v>
+      </c>
+      <c r="C33">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="2">
+        <v>44225.083333159724</v>
+      </c>
+      <c r="B34">
+        <v>20</v>
+      </c>
+      <c r="C34">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" s="2">
+        <v>44226.083333159724</v>
+      </c>
+      <c r="B35">
+        <v>20</v>
+      </c>
+      <c r="C35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="2">
+        <v>44227.083333159724</v>
+      </c>
+      <c r="B36">
+        <v>20</v>
+      </c>
+      <c r="C36">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="2">
+        <v>44228.083333159724</v>
+      </c>
+      <c r="B37">
+        <v>20</v>
+      </c>
+      <c r="C37">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" s="2">
+        <v>44229.083333159724</v>
+      </c>
+      <c r="B38">
+        <v>20</v>
+      </c>
+      <c r="C38">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" s="2">
+        <v>44230.083333159724</v>
+      </c>
+      <c r="B39">
+        <v>20</v>
+      </c>
+      <c r="C39">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" s="2">
+        <v>44231.083333159724</v>
+      </c>
+      <c r="B40">
+        <v>20</v>
+      </c>
+      <c r="C40">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" s="2">
+        <v>44232.083333159724</v>
+      </c>
+      <c r="B41">
+        <v>20</v>
+      </c>
+      <c r="C41">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" s="2">
+        <v>44233.083333159724</v>
+      </c>
+      <c r="B42">
+        <v>20</v>
+      </c>
+      <c r="C42">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" s="2">
+        <v>44234.083333159724</v>
+      </c>
+      <c r="B43">
+        <v>20</v>
+      </c>
+      <c r="C43">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" s="2">
+        <v>44235.083333159724</v>
+      </c>
+      <c r="B44">
+        <v>20</v>
+      </c>
+      <c r="C44">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" s="2">
+        <v>44236.083333159724</v>
+      </c>
+      <c r="B45">
+        <v>20</v>
+      </c>
+      <c r="C45">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" s="2">
+        <v>44237.083333159724</v>
+      </c>
+      <c r="B46">
+        <v>20</v>
+      </c>
+      <c r="C46">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" s="2">
+        <v>44238.083333159724</v>
+      </c>
+      <c r="B47">
+        <v>20</v>
+      </c>
+      <c r="C47">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48" s="2">
+        <v>44239.083333159724</v>
+      </c>
+      <c r="B48">
+        <v>20</v>
+      </c>
+      <c r="C48">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" s="2">
+        <v>44240.083333159724</v>
+      </c>
+      <c r="B49">
+        <v>20</v>
+      </c>
+      <c r="C49">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50" s="2">
+        <v>44241.083333159724</v>
+      </c>
+      <c r="B50">
+        <v>20</v>
+      </c>
+      <c r="C50">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" s="2">
+        <v>44242.083333159724</v>
+      </c>
+      <c r="B51">
+        <v>20</v>
+      </c>
+      <c r="C51">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" s="2">
+        <v>44243.083333159724</v>
+      </c>
+      <c r="B52">
+        <v>20</v>
+      </c>
+      <c r="C52">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53" s="2">
+        <v>44244.083333159724</v>
+      </c>
+      <c r="B53">
+        <v>20</v>
+      </c>
+      <c r="C53">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54" s="2">
+        <v>44245.083333159724</v>
+      </c>
+      <c r="B54">
+        <v>20</v>
+      </c>
+      <c r="C54">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" s="2"/>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" s="2"/>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" s="2"/>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" s="2"/>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" s="2"/>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" s="2"/>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" s="2"/>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" s="2"/>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" s="2"/>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" s="2"/>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Loaded all the changes to test input and test scripts
</commit_message>
<xml_diff>
--- a/eureca_dhcs/test/input_tests/conditions_hydro_test_2.xlsx
+++ b/eureca_dhcs/test/input_tests/conditions_hydro_test_2.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20386"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDB37DFA-D292-4367-BB1A-51FEC9C273AA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24CB9FE5-4FA2-49C7-BAB1-C624805150F2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21528" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="23400" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hydraulic" sheetId="1" r:id="rId1"/>
@@ -366,8 +366,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J8763"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="D51" sqref="D51"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -807,22 +807,22 @@
         <v>44207.083333159724</v>
       </c>
       <c r="B16" s="3">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="C16" s="3">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="D16" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E16" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F16" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G16" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
@@ -830,22 +830,22 @@
         <v>44208.083333159724</v>
       </c>
       <c r="B17" s="3">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="C17" s="3">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="D17" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E17" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F17" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G17" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
@@ -853,22 +853,22 @@
         <v>44209.083333159724</v>
       </c>
       <c r="B18" s="3">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="C18" s="3">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="D18" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E18" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F18" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G18" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
@@ -876,22 +876,22 @@
         <v>44210.083333159724</v>
       </c>
       <c r="B19" s="3">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="C19" s="3">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="D19" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E19" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F19" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G19" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
@@ -899,22 +899,22 @@
         <v>44211.083333159724</v>
       </c>
       <c r="B20" s="3">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="C20" s="3">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="D20" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E20" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F20" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G20" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
@@ -922,22 +922,22 @@
         <v>44212.083333159724</v>
       </c>
       <c r="B21" s="3">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="C21" s="3">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="D21" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E21" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F21" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G21" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
@@ -945,22 +945,22 @@
         <v>44213.083333159724</v>
       </c>
       <c r="B22" s="3">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="C22" s="3">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="D22" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E22" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F22" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G22" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
@@ -968,22 +968,22 @@
         <v>44214.083333159724</v>
       </c>
       <c r="B23" s="3">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="C23" s="3">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="D23" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E23" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F23" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G23" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
@@ -991,22 +991,22 @@
         <v>44215.083333159724</v>
       </c>
       <c r="B24" s="3">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="C24" s="3">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="D24" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E24" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F24" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G24" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
@@ -1014,22 +1014,22 @@
         <v>44216.083333159724</v>
       </c>
       <c r="B25" s="3">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="C25" s="3">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="D25" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E25" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F25" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G25" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
@@ -1037,22 +1037,22 @@
         <v>44217.083333159724</v>
       </c>
       <c r="B26" s="3">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="C26" s="3">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="D26" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E26" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F26" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G26" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
@@ -1060,22 +1060,22 @@
         <v>44218.083333159724</v>
       </c>
       <c r="B27" s="3">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="C27" s="3">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="D27" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E27" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F27" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G27" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
@@ -1083,22 +1083,22 @@
         <v>44219.083333159724</v>
       </c>
       <c r="B28" s="3">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="C28" s="3">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="D28" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E28" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F28" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G28" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
@@ -1106,22 +1106,22 @@
         <v>44220.083333159724</v>
       </c>
       <c r="B29" s="3">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="C29" s="3">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="D29" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E29" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F29" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G29" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
@@ -1166,11 +1166,11 @@
         <v>-34.889400000000002</v>
       </c>
       <c r="D31" s="3">
-        <f t="shared" ref="D31:D54" si="9">113.4/3.6*0.994*2</f>
+        <f t="shared" ref="D31:D43" si="9">113.4/3.6*0.994*2</f>
         <v>62.622</v>
       </c>
       <c r="E31" s="3">
-        <f t="shared" ref="E31:E54" si="10">90.72/3.6*0.994/2</f>
+        <f t="shared" ref="E31:E43" si="10">90.72/3.6*0.994/2</f>
         <v>12.5244</v>
       </c>
       <c r="F31" s="3">

</xml_diff>